<commit_message>
Updates to boxplots. Generate shapley owen plots. Other organization.
</commit_message>
<xml_diff>
--- a/output/20221121/tables/variance_decomposition/variance_decomposition.xlsx
+++ b/output/20221121/tables/variance_decomposition/variance_decomposition.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="44">
   <si>
     <t>Outcome</t>
   </si>
@@ -191,7 +191,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L31"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -310,610 +310,1066 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
-        <v>0.18335311114788055</v>
+        <v>0.14611367881298065</v>
       </c>
       <c r="D4" s="1">
-        <v>0.051559984683990479</v>
+        <v>0.16299311816692352</v>
       </c>
       <c r="E4" s="1">
-        <v>0.049298565834760666</v>
+        <v>0.094275817275047302</v>
       </c>
       <c r="F4" s="1">
-        <v>0.0013610448222607374</v>
+        <v>0.0039873383939266205</v>
       </c>
       <c r="G4" s="1">
-        <v>0.0018599035684019327</v>
+        <v>0.0083868298679590225</v>
       </c>
       <c r="H4" s="1">
-        <v>0.0010245206067338586</v>
+        <v>0.0034284086432307959</v>
       </c>
       <c r="I4" s="1">
-        <v>0.0014570518396794796</v>
+        <v>0.018397277221083641</v>
       </c>
       <c r="J4" s="1">
-        <v>0.0036468759644776583</v>
+        <v>0.002615851815789938</v>
       </c>
       <c r="K4" s="1">
-        <v>0.0014818365452811122</v>
+        <v>0.026472894474864006</v>
       </c>
       <c r="L4" s="1">
-        <v>0.29504290223121643</v>
+        <v>0.46667122840881348</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>0.022374870255589485</v>
+        <v>0.18335311114788055</v>
       </c>
       <c r="D5" s="1">
-        <v>0.062917008996009827</v>
+        <v>0.051559984683990479</v>
       </c>
       <c r="E5" s="1">
-        <v>0.034494441002607346</v>
+        <v>0.049298565834760666</v>
       </c>
       <c r="F5" s="1">
-        <v>0.00826299749314785</v>
+        <v>0.0013610448222607374</v>
       </c>
       <c r="G5" s="1">
-        <v>0.0016223450656980276</v>
+        <v>0.0018599035684019327</v>
       </c>
       <c r="H5" s="1">
-        <v>0.0062972088344395161</v>
+        <v>0.0010245206067338586</v>
       </c>
       <c r="I5" s="1">
-        <v>0.0065514813177287579</v>
+        <v>0.0014570518396794796</v>
       </c>
       <c r="J5" s="1">
-        <v>0.00022513518342748284</v>
+        <v>0.0036468759644776583</v>
       </c>
       <c r="K5" s="1">
-        <v>0.0046687237918376923</v>
+        <v>0.0014818365452811122</v>
       </c>
       <c r="L5" s="1">
-        <v>0.14741420745849609</v>
+        <v>0.29504290223121643</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>0.50414896011352539</v>
+        <v>0.019214589148759842</v>
       </c>
       <c r="D6" s="1">
-        <v>0.020393695682287216</v>
+        <v>0.076772153377532959</v>
       </c>
       <c r="E6" s="1">
-        <v>0.01096759270876646</v>
+        <v>0.065931655466556549</v>
       </c>
       <c r="F6" s="1">
-        <v>0.0026122282724827528</v>
+        <v>0.0021918998099863529</v>
       </c>
       <c r="G6" s="1">
-        <v>0.0039442009292542934</v>
+        <v>0.0023248984944075346</v>
       </c>
       <c r="H6" s="1">
-        <v>0.0096150543540716171</v>
+        <v>0.0010870638070628047</v>
       </c>
       <c r="I6" s="1">
-        <v>0.00083914585411548615</v>
+        <v>6.9245346821844578e-05</v>
       </c>
       <c r="J6" s="1">
-        <v>0.00024779254454188049</v>
+        <v>0.0034090855624526739</v>
       </c>
       <c r="K6" s="1">
-        <v>0.00085708749247714877</v>
+        <v>0.00037484642234630883</v>
       </c>
       <c r="L6" s="1">
-        <v>0.55362576246261597</v>
+        <v>0.17137543857097626</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
-        <v>0.54859566688537598</v>
+        <v>0.022374870255589485</v>
       </c>
       <c r="D7" s="1">
-        <v>0.015247498638927937</v>
+        <v>0.062917008996009827</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0098018525168299675</v>
+        <v>0.034494441002607346</v>
       </c>
       <c r="F7" s="1">
-        <v>0.0014782128855586052</v>
+        <v>0.00826299749314785</v>
       </c>
       <c r="G7" s="1">
-        <v>0.00047882151557132602</v>
+        <v>0.0016223450656980276</v>
       </c>
       <c r="H7" s="1">
-        <v>0.0015336424112319946</v>
+        <v>0.0062972088344395161</v>
       </c>
       <c r="I7" s="1">
-        <v>0.0019499941263347864</v>
+        <v>0.0065514813177287579</v>
       </c>
       <c r="J7" s="1">
-        <v>0.0012283520773053169</v>
+        <v>0.00022513518342748284</v>
       </c>
       <c r="K7" s="1">
-        <v>0.0066126659512519836</v>
+        <v>0.0046687237918376923</v>
       </c>
       <c r="L7" s="1">
-        <v>0.58692669868469238</v>
+        <v>0.14741420745849609</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>0.010484673082828522</v>
+        <v>0.50414896011352539</v>
       </c>
       <c r="D8" s="1">
-        <v>0.001827630796469748</v>
+        <v>0.020393695682287216</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0035333596169948578</v>
+        <v>0.01096759270876646</v>
       </c>
       <c r="F8" s="1">
-        <v>0.0019468403188511729</v>
+        <v>0.0026122282724827528</v>
       </c>
       <c r="G8" s="1">
-        <v>0.0089301168918609619</v>
+        <v>0.0039442009292542934</v>
       </c>
       <c r="H8" s="1">
-        <v>0.0060300002805888653</v>
+        <v>0.0096150543540716171</v>
       </c>
       <c r="I8" s="1">
-        <v>0.0034771019127219915</v>
+        <v>0.00083914585411548615</v>
       </c>
       <c r="J8" s="1">
-        <v>0.010004214942455292</v>
+        <v>0.00024779254454188049</v>
       </c>
       <c r="K8" s="1">
-        <v>0.009251616895198822</v>
+        <v>0.00085708749247714877</v>
       </c>
       <c r="L8" s="1">
-        <v>0.055485554039478302</v>
+        <v>0.55362576246261597</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
-        <v>0.71178394556045532</v>
+        <v>0.018675506114959717</v>
       </c>
       <c r="D9" s="1">
-        <v>0.0044683124870061874</v>
+        <v>0.040833450853824615</v>
       </c>
       <c r="E9" s="1">
-        <v>0.006861124187707901</v>
+        <v>0.020213587209582329</v>
       </c>
       <c r="F9" s="1">
-        <v>0.001293676788918674</v>
+        <v>0.0044605578295886517</v>
       </c>
       <c r="G9" s="1">
-        <v>0.0050563360564410686</v>
+        <v>0.0056543881073594093</v>
       </c>
       <c r="H9" s="1">
-        <v>0.0029094673227518797</v>
+        <v>0.01340862549841404</v>
       </c>
       <c r="I9" s="1">
-        <v>0.0020077344961464405</v>
+        <v>0.0005061004776507616</v>
       </c>
       <c r="J9" s="1">
-        <v>0.013907885178923607</v>
+        <v>0.00024376032524742186</v>
       </c>
       <c r="K9" s="1">
-        <v>0.0056905210949480534</v>
+        <v>0.00021977403957862407</v>
       </c>
       <c r="L9" s="1">
-        <v>0.75397902727127075</v>
+        <v>0.10421574860811234</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>0.19075565040111542</v>
+        <v>0.54859566688537598</v>
       </c>
       <c r="D10" s="1">
-        <v>0.061788816004991531</v>
+        <v>0.015247498638927937</v>
       </c>
       <c r="E10" s="1">
-        <v>0.031240105628967285</v>
+        <v>0.0098018525168299675</v>
       </c>
       <c r="F10" s="1">
-        <v>0.0010046280222013593</v>
+        <v>0.0014782128855586052</v>
       </c>
       <c r="G10" s="1">
-        <v>0.0073042041622102261</v>
+        <v>0.00047882151557132602</v>
       </c>
       <c r="H10" s="1">
-        <v>0.0016164684202522039</v>
+        <v>0.0015336424112319946</v>
       </c>
       <c r="I10" s="1">
-        <v>0.0019155374029651284</v>
+        <v>0.0019499941263347864</v>
       </c>
       <c r="J10" s="1">
-        <v>0.0013623811537399888</v>
+        <v>0.0012283520773053169</v>
       </c>
       <c r="K10" s="1">
-        <v>0.0042006787844002247</v>
+        <v>0.0066126659512519836</v>
       </c>
       <c r="L10" s="1">
-        <v>0.30118846893310547</v>
+        <v>0.58692669868469238</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
-        <v>0.08790896087884903</v>
+        <v>0.0049590221606194973</v>
       </c>
       <c r="D11" s="1">
-        <v>0.01577288843691349</v>
+        <v>0.027450237423181534</v>
       </c>
       <c r="E11" s="1">
-        <v>0.0078019234351813793</v>
+        <v>0.015791045501828194</v>
       </c>
       <c r="F11" s="1">
-        <v>0.00096181238768622279</v>
+        <v>0.0012595112202689052</v>
       </c>
       <c r="G11" s="1">
-        <v>0.0035624781157821417</v>
+        <v>0.00085011031478643417</v>
       </c>
       <c r="H11" s="1">
-        <v>0.0027882035356014967</v>
+        <v>0.0024704416282474995</v>
       </c>
       <c r="I11" s="1">
-        <v>0.004349900409579277</v>
+        <v>0.0039582042954862118</v>
       </c>
       <c r="J11" s="1">
-        <v>0.010393508709967136</v>
+        <v>0.0011653861729428172</v>
       </c>
       <c r="K11" s="1">
-        <v>0.0080069340765476227</v>
+        <v>0.010884913615882397</v>
       </c>
       <c r="L11" s="1">
-        <v>0.14154660701751709</v>
+        <v>0.068788871169090271</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
-        <v>0.72599989175796509</v>
+        <v>0.010484673082828522</v>
       </c>
       <c r="D12" s="1">
-        <v>0.010595472529530525</v>
+        <v>0.001827630796469748</v>
       </c>
       <c r="E12" s="1">
-        <v>0.0066133732907474041</v>
+        <v>0.0035333596169948578</v>
       </c>
       <c r="F12" s="1">
-        <v>0.0017821019282564521</v>
+        <v>0.0019468403188511729</v>
       </c>
       <c r="G12" s="1">
-        <v>0.0051918369717895985</v>
+        <v>0.0089301168918609619</v>
       </c>
       <c r="H12" s="1">
-        <v>0.0011350295972079039</v>
+        <v>0.0060300002805888653</v>
       </c>
       <c r="I12" s="1">
-        <v>0.002540254732593894</v>
+        <v>0.0034771019127219915</v>
       </c>
       <c r="J12" s="1">
-        <v>0.0057392236776649952</v>
+        <v>0.010004214942455292</v>
       </c>
       <c r="K12" s="1">
-        <v>0.0023070052266120911</v>
+        <v>0.009251616895198822</v>
       </c>
       <c r="L12" s="1">
-        <v>0.76190418004989624</v>
+        <v>0.055485554039478302</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>0.025809368118643761</v>
+        <v>0.71178394556045532</v>
       </c>
       <c r="D13" s="1">
-        <v>0.098223753273487091</v>
+        <v>0.0044683124870061874</v>
       </c>
       <c r="E13" s="1">
-        <v>0.051046606153249741</v>
+        <v>0.006861124187707901</v>
       </c>
       <c r="F13" s="1">
-        <v>0.0028725042939186096</v>
+        <v>0.001293676788918674</v>
       </c>
       <c r="G13" s="1">
-        <v>0.0045543941669166088</v>
+        <v>0.0050563360564410686</v>
       </c>
       <c r="H13" s="1">
-        <v>0.00052294041961431503</v>
+        <v>0.0029094673227518797</v>
       </c>
       <c r="I13" s="1">
-        <v>0.0016962020890787244</v>
+        <v>0.0020077344961464405</v>
       </c>
       <c r="J13" s="1">
-        <v>0.007146280724555254</v>
+        <v>0.013907885178923607</v>
       </c>
       <c r="K13" s="1">
-        <v>0.0030542302411049604</v>
+        <v>0.0056905210949480534</v>
       </c>
       <c r="L13" s="1">
-        <v>0.19492627680301666</v>
+        <v>0.75397902727127075</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>0.097390376031398773</v>
+        <v>0.015686102211475372</v>
       </c>
       <c r="D14" s="1">
-        <v>0.083254098892211914</v>
+        <v>0.005917754489928484</v>
       </c>
       <c r="E14" s="1">
-        <v>0.043326131999492645</v>
+        <v>0.010494755581021309</v>
       </c>
       <c r="F14" s="1">
-        <v>0.0043195602484047413</v>
+        <v>0.0013577275676652789</v>
       </c>
       <c r="G14" s="1">
-        <v>0.013548612594604492</v>
+        <v>0.0080954888835549355</v>
       </c>
       <c r="H14" s="1">
-        <v>0.0094074932858347893</v>
+        <v>0.0047463793307542801</v>
       </c>
       <c r="I14" s="1">
-        <v>0.015302481129765511</v>
+        <v>0.0044012945145368576</v>
       </c>
       <c r="J14" s="1">
-        <v>0.0036599428858608007</v>
+        <v>0.021927377209067345</v>
       </c>
       <c r="K14" s="1">
-        <v>0.020174402743577957</v>
+        <v>0.00096030934946611524</v>
       </c>
       <c r="L14" s="1">
-        <v>0.29038310050964355</v>
+        <v>0.073587186634540558</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>0.74949914216995239</v>
+        <v>0.19075565040111542</v>
       </c>
       <c r="D15" s="1">
-        <v>0.066129051148891449</v>
+        <v>0.061788816004991531</v>
       </c>
       <c r="E15" s="1">
-        <v>0.03661452978849411</v>
+        <v>0.031240105628967285</v>
       </c>
       <c r="F15" s="1">
-        <v>0.0015250128926709294</v>
+        <v>0.0010046280222013593</v>
       </c>
       <c r="G15" s="1">
-        <v>0.0066790636628866196</v>
+        <v>0.0073042041622102261</v>
       </c>
       <c r="H15" s="1">
-        <v>0.0058778133243322372</v>
+        <v>0.0016164684202522039</v>
       </c>
       <c r="I15" s="1">
-        <v>0.0083910766988992691</v>
+        <v>0.0019155374029651284</v>
       </c>
       <c r="J15" s="1">
-        <v>0.0011355932801961899</v>
+        <v>0.0013623811537399888</v>
       </c>
       <c r="K15" s="1">
-        <v>0.0077096465975046158</v>
+        <v>0.0042006787844002247</v>
       </c>
       <c r="L15" s="1">
-        <v>0.88356095552444458</v>
+        <v>0.30118846893310547</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
-        <v>0.06586100161075592</v>
+        <v>0.0059019518084824085</v>
       </c>
       <c r="D16" s="1">
-        <v>0.082496009767055511</v>
+        <v>0.062952011823654175</v>
       </c>
       <c r="E16" s="1">
-        <v>0.055036198347806931</v>
+        <v>0.031556915491819382</v>
       </c>
       <c r="F16" s="1">
-        <v>0.004235757514834404</v>
+        <v>0.0010806946083903313</v>
       </c>
       <c r="G16" s="1">
-        <v>0.0019773859530687332</v>
+        <v>0.0099254585802555084</v>
       </c>
       <c r="H16" s="1">
-        <v>0.0021507011260837317</v>
+        <v>0.0026653429958969355</v>
       </c>
       <c r="I16" s="1">
-        <v>0.0004460006020963192</v>
+        <v>0.00082494539674371481</v>
       </c>
       <c r="J16" s="1">
-        <v>0.0066573102958500385</v>
+        <v>0.00025381494197063148</v>
       </c>
       <c r="K16" s="1">
-        <v>0.00063556531677022576</v>
+        <v>0.0063988901674747467</v>
       </c>
       <c r="L16" s="1">
-        <v>0.21949593722820282</v>
+        <v>0.12156002223491669</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
-        <v>0.014397848397493362</v>
+        <v>0.08790896087884903</v>
       </c>
       <c r="D17" s="1">
-        <v>0.052001137286424637</v>
+        <v>0.01577288843691349</v>
       </c>
       <c r="E17" s="1">
-        <v>0.02536316029727459</v>
+        <v>0.0078019234351813793</v>
       </c>
       <c r="F17" s="1">
-        <v>0.0030153687112033367</v>
+        <v>0.00096181238768622279</v>
       </c>
       <c r="G17" s="1">
-        <v>0.0059853033162653446</v>
+        <v>0.0035624781157821417</v>
       </c>
       <c r="H17" s="1">
-        <v>0.015011833049356937</v>
+        <v>0.0027882035356014967</v>
       </c>
       <c r="I17" s="1">
-        <v>0.012273287400603294</v>
+        <v>0.004349900409579277</v>
       </c>
       <c r="J17" s="1">
-        <v>0.0053963325917720795</v>
+        <v>0.010393508709967136</v>
       </c>
       <c r="K17" s="1">
-        <v>0.02022012323141098</v>
+        <v>0.0080069340765476227</v>
       </c>
       <c r="L17" s="1">
-        <v>0.15366439521312714</v>
+        <v>0.14154660701751709</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1">
-        <v>0.67653471231460571</v>
+        <v>0.72599989175796509</v>
       </c>
       <c r="D18" s="1">
-        <v>0.046808473765850067</v>
+        <v>0.010595472529530525</v>
       </c>
       <c r="E18" s="1">
-        <v>0.023864112794399261</v>
+        <v>0.0066133732907474041</v>
       </c>
       <c r="F18" s="1">
-        <v>0.00090107100550085306</v>
+        <v>0.0017821019282564521</v>
       </c>
       <c r="G18" s="1">
-        <v>0.0024983477778732777</v>
+        <v>0.0051918369717895985</v>
       </c>
       <c r="H18" s="1">
-        <v>0.0055537540465593338</v>
+        <v>0.0011350295972079039</v>
       </c>
       <c r="I18" s="1">
-        <v>0.0066236937418580055</v>
+        <v>0.002540254732593894</v>
       </c>
       <c r="J18" s="1">
-        <v>0.00093886529793962836</v>
+        <v>0.0057392236776649952</v>
       </c>
       <c r="K18" s="1">
-        <v>0.0060328678227961063</v>
+        <v>0.0023070052266120911</v>
       </c>
       <c r="L18" s="1">
-        <v>0.76975589990615845</v>
+        <v>0.76190418004989624</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.068091869354248047</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.021542361006140709</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.011900738812983036</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.0019258500542491674</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.005994593258947134</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.0012448689667508006</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.0048354603350162506</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.0088800918310880661</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.0013429059181362391</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.12575873732566833</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.025809368118643761</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.098223753273487091</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.051046606153249741</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.0028725042939186096</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.0045543941669166088</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.00052294041961431503</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.0016962020890787244</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.007146280724555254</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.0030542302411049604</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.19492627680301666</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.0013740187278017402</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.10390001535415649</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.053449623286724091</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.0029899063520133495</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.004102607723325491</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.00040726966108195484</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.0013305904576554894</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.0083929877728223801</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.0024810787290334702</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.17842809855937958</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.097390376031398773</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.083254098892211914</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.043326131999492645</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.0043195602484047413</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.013548612594604492</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.0094074932858347893</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.015302481129765511</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.0036599428858608007</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.020174402743577957</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.29038310050964355</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.74949914216995239</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.066129051148891449</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.03661452978849411</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.0015250128926709294</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.0066790636628866196</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.0058778133243322372</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.0083910766988992691</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.0011355932801961899</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.0077096465975046158</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.88356095552444458</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.093720801174640656</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.1159827709197998</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.059968046844005585</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.0042141708545386791</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.011401458643376827</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.0072210482321679592</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.014926867559552193</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.0008675925200805068</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.013185835443437099</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.32148858904838562</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.06586100161075592</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.082496009767055511</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.055036198347806931</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.004235757514834404</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.0019773859530687332</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.0021507011260837317</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.0004460006020963192</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.0066573102958500385</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.00063556531677022576</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.21949593722820282</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.0016227908199653029</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.10004986077547073</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.064199239015579224</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.0052248700521886349</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.0010353946126997471</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.0028678036760538816</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.00010479483898961917</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.0079850032925605774</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.00053984799887984991</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.1836296021938324</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.014397848397493362</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.052001137286424637</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.02536316029727459</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.0030153687112033367</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.0059853033162653446</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.015011833049356937</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.012273287400603294</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.0053963325917720795</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.02022012323141098</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.15366439521312714</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.67653471231460571</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.046808473765850067</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.023864112794399261</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.00090107100550085306</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.0024983477778732777</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.0055537540465593338</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.0066236937418580055</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.00093886529793962836</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.0060328678227961063</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0.76975589990615845</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.019071068614721298</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.080812811851501465</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.039758197963237762</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.0027485722675919533</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.0052555329166352749</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.0089209806174039841</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.012444166466593742</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.0014040968380868435</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.0083658294752240181</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.17878125607967377</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C30" s="1">
         <v>0.04363519698381424</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D30" s="1">
         <v>0.033326920121908188</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E30" s="1">
         <v>0.017105609178543091</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F30" s="1">
         <v>0.0019501224160194397</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G30" s="1">
         <v>0.0020112611819058657</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H30" s="1">
         <v>0.0015578551683574915</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I30" s="1">
         <v>0.00067801907425746322</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J30" s="1">
         <v>0.00041312372195534408</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K30" s="1">
         <v>0.006496489979326725</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L30" s="1">
         <v>0.1071745976805687</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.0005015972419641912</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.024197202175855637</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.012461387552320957</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.0024035670794546604</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.0029436692129820585</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.0028141320217400789</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.00014485725841950625</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.00010717324039433151</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.0092304050922393799</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.054803989827632904</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +1378,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H31"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1005,418 +1461,730 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
-        <v>0.20127114653587341</v>
+        <v>0.14162507653236389</v>
       </c>
       <c r="D4" s="1">
-        <v>0.082795754075050354</v>
+        <v>0.26161155104637146</v>
       </c>
       <c r="E4" s="1">
-        <v>0.0044297906570136547</v>
+        <v>0.015972089022397995</v>
       </c>
       <c r="F4" s="1">
-        <v>0.0050244256854057312</v>
+        <v>0.020388785749673843</v>
       </c>
       <c r="G4" s="1">
-        <v>0.0015217799227684736</v>
+        <v>0.02707374095916748</v>
       </c>
       <c r="H4" s="1">
-        <v>0.29504290223121643</v>
+        <v>0.46667122840881348</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>0.022044051438570023</v>
+        <v>0.20127114653587341</v>
       </c>
       <c r="D5" s="1">
-        <v>0.095593616366386414</v>
+        <v>0.082795754075050354</v>
       </c>
       <c r="E5" s="1">
-        <v>0.017875213176012039</v>
+        <v>0.0044297906570136547</v>
       </c>
       <c r="F5" s="1">
-        <v>0.0070331520400941372</v>
+        <v>0.0050244256854057312</v>
       </c>
       <c r="G5" s="1">
-        <v>0.0048681716434657574</v>
+        <v>0.0015217799227684736</v>
       </c>
       <c r="H5" s="1">
-        <v>0.14741420745849609</v>
+        <v>0.29504290223121643</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>0.50524169206619263</v>
+        <v>0.018043037503957748</v>
       </c>
       <c r="D6" s="1">
-        <v>0.028998944908380508</v>
+        <v>0.14398933947086334</v>
       </c>
       <c r="E6" s="1">
-        <v>0.017357118427753448</v>
+        <v>0.0057175289839506149</v>
       </c>
       <c r="F6" s="1">
-        <v>0.0011418814538046718</v>
+        <v>0.0031528121326118708</v>
       </c>
       <c r="G6" s="1">
-        <v>0.00088610698003321886</v>
+        <v>0.00047272746451199055</v>
       </c>
       <c r="H6" s="1">
-        <v>0.55362576246261597</v>
+        <v>0.17137543857097626</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
-        <v>0.55232489109039307</v>
+        <v>0.022044051438570023</v>
       </c>
       <c r="D7" s="1">
-        <v>0.020620228722691536</v>
+        <v>0.095593616366386414</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0039409794844686985</v>
+        <v>0.017875213176012039</v>
       </c>
       <c r="F7" s="1">
-        <v>0.0034384001046419144</v>
+        <v>0.0070331520400941372</v>
       </c>
       <c r="G7" s="1">
-        <v>0.0066021895036101341</v>
+        <v>0.0048681716434657574</v>
       </c>
       <c r="H7" s="1">
-        <v>0.58692669868469238</v>
+        <v>0.14741420745849609</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>0.010576654225587845</v>
+        <v>0.50524169206619263</v>
       </c>
       <c r="D8" s="1">
-        <v>0.0052544255740940571</v>
+        <v>0.028998944908380508</v>
       </c>
       <c r="E8" s="1">
-        <v>0.016525860875844955</v>
+        <v>0.017357118427753448</v>
       </c>
       <c r="F8" s="1">
-        <v>0.013671423308551311</v>
+        <v>0.0011418814538046718</v>
       </c>
       <c r="G8" s="1">
-        <v>0.0094571895897388458</v>
+        <v>0.00088610698003321886</v>
       </c>
       <c r="H8" s="1">
-        <v>0.055485554039478302</v>
+        <v>0.55362576246261597</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
-        <v>0.71174675226211548</v>
+        <v>0.018644360825419426</v>
       </c>
       <c r="D9" s="1">
-        <v>0.011219686828553677</v>
+        <v>0.060216844081878662</v>
       </c>
       <c r="E9" s="1">
-        <v>0.0090767238289117813</v>
+        <v>0.024172458797693253</v>
       </c>
       <c r="F9" s="1">
-        <v>0.01641002856194973</v>
+        <v>0.00086683331755921245</v>
       </c>
       <c r="G9" s="1">
-        <v>0.0055258539505302906</v>
+        <v>0.00031525420490652323</v>
       </c>
       <c r="H9" s="1">
-        <v>0.75397902727127075</v>
+        <v>0.10421574860811234</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>0.18809676170349121</v>
+        <v>0.55232489109039307</v>
       </c>
       <c r="D10" s="1">
-        <v>0.095124803483486176</v>
+        <v>0.020620228722691536</v>
       </c>
       <c r="E10" s="1">
-        <v>0.010704449377954006</v>
+        <v>0.0039409794844686985</v>
       </c>
       <c r="F10" s="1">
-        <v>0.0028809099458158016</v>
+        <v>0.0034384001046419144</v>
       </c>
       <c r="G10" s="1">
-        <v>0.0043815341778099537</v>
+        <v>0.0066021895036101341</v>
       </c>
       <c r="H10" s="1">
-        <v>0.30118846893310547</v>
+        <v>0.58692669868469238</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
-        <v>0.086055271327495575</v>
+        <v>0.0048333704471588135</v>
       </c>
       <c r="D11" s="1">
-        <v>0.025239139795303345</v>
+        <v>0.042670451104640961</v>
       </c>
       <c r="E11" s="1">
-        <v>0.0073612192645668983</v>
+        <v>0.005035878624767065</v>
       </c>
       <c r="F11" s="1">
-        <v>0.014970019459724426</v>
+        <v>0.0053192027844488621</v>
       </c>
       <c r="G11" s="1">
-        <v>0.0079209562391042709</v>
+        <v>0.010929970070719719</v>
       </c>
       <c r="H11" s="1">
-        <v>0.14154660701751709</v>
+        <v>0.068788871169090271</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
-        <v>0.72759950160980225</v>
+        <v>0.010576654225587845</v>
       </c>
       <c r="D12" s="1">
-        <v>0.015304251573979855</v>
+        <v>0.0052544255740940571</v>
       </c>
       <c r="E12" s="1">
-        <v>0.0078181307762861252</v>
+        <v>0.016525860875844955</v>
       </c>
       <c r="F12" s="1">
-        <v>0.0089204329997301102</v>
+        <v>0.013671423308551311</v>
       </c>
       <c r="G12" s="1">
-        <v>0.0022618710063397884</v>
+        <v>0.0094571895897388458</v>
       </c>
       <c r="H12" s="1">
-        <v>0.76190418004989624</v>
+        <v>0.055485554039478302</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>0.026782017201185226</v>
+        <v>0.71174675226211548</v>
       </c>
       <c r="D13" s="1">
-        <v>0.14786736667156219</v>
+        <v>0.011219686828553677</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0079238424077630043</v>
+        <v>0.0090767238289117813</v>
       </c>
       <c r="F13" s="1">
-        <v>0.0089279608801007271</v>
+        <v>0.01641002856194973</v>
       </c>
       <c r="G13" s="1">
-        <v>0.0034250891767442226</v>
+        <v>0.0055258539505302906</v>
       </c>
       <c r="H13" s="1">
-        <v>0.19492627680301666</v>
+        <v>0.75397902727127075</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>0.095474287867546082</v>
+        <v>0.01553007960319519</v>
       </c>
       <c r="D14" s="1">
-        <v>0.12921270728111267</v>
+        <v>0.017371395602822304</v>
       </c>
       <c r="E14" s="1">
-        <v>0.02707943320274353</v>
+        <v>0.013753321953117847</v>
       </c>
       <c r="F14" s="1">
-        <v>0.018484009429812431</v>
+        <v>0.026178926229476929</v>
       </c>
       <c r="G14" s="1">
-        <v>0.02013266459107399</v>
+        <v>0.00075346388621255755</v>
       </c>
       <c r="H14" s="1">
-        <v>0.29038310050964355</v>
+        <v>0.073587186634540558</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>0.75850707292556763</v>
+        <v>0.18809676170349121</v>
       </c>
       <c r="D15" s="1">
-        <v>0.093052171170711517</v>
+        <v>0.095124803483486176</v>
       </c>
       <c r="E15" s="1">
-        <v>0.01492936909198761</v>
+        <v>0.010704449377954006</v>
       </c>
       <c r="F15" s="1">
-        <v>0.009319760836660862</v>
+        <v>0.0028809099458158016</v>
       </c>
       <c r="G15" s="1">
-        <v>0.0077525991946458817</v>
+        <v>0.0043815341778099537</v>
       </c>
       <c r="H15" s="1">
-        <v>0.88356095552444458</v>
+        <v>0.30118846893310547</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
-        <v>0.072957605123519897</v>
+        <v>0.0065471655689179897</v>
       </c>
       <c r="D16" s="1">
-        <v>0.13023675978183746</v>
+        <v>0.093354947865009308</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0086859436705708504</v>
+        <v>0.014085313305258751</v>
       </c>
       <c r="F16" s="1">
-        <v>0.0068710003979504108</v>
+        <v>0.00098150852136313915</v>
       </c>
       <c r="G16" s="1">
-        <v>0.00074462429620325565</v>
+        <v>0.0065910876728594303</v>
       </c>
       <c r="H16" s="1">
-        <v>0.21949593722820282</v>
+        <v>0.12156002223491669</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
-        <v>0.013937021605670452</v>
+        <v>0.086055271327495575</v>
       </c>
       <c r="D17" s="1">
-        <v>0.078382425010204315</v>
+        <v>0.025239139795303345</v>
       </c>
       <c r="E17" s="1">
-        <v>0.024353647604584694</v>
+        <v>0.0073612192645668983</v>
       </c>
       <c r="F17" s="1">
-        <v>0.017090862616896629</v>
+        <v>0.014970019459724426</v>
       </c>
       <c r="G17" s="1">
-        <v>0.01990043930709362</v>
+        <v>0.0079209562391042709</v>
       </c>
       <c r="H17" s="1">
-        <v>0.15366439521312714</v>
+        <v>0.14154660701751709</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1">
-        <v>0.67860984802246094</v>
+        <v>0.72759950160980225</v>
       </c>
       <c r="D18" s="1">
-        <v>0.06802792102098465</v>
+        <v>0.015304251573979855</v>
       </c>
       <c r="E18" s="1">
-        <v>0.0096436068415641785</v>
+        <v>0.0078181307762861252</v>
       </c>
       <c r="F18" s="1">
-        <v>0.0074772806838154793</v>
+        <v>0.0089204329997301102</v>
       </c>
       <c r="G18" s="1">
-        <v>0.0059972428716719151</v>
+        <v>0.0022618710063397884</v>
       </c>
       <c r="H18" s="1">
-        <v>0.76975589990615845</v>
+        <v>0.76190418004989624</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.066197790205478668</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.035362664610147476</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.0089181065559387207</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.0139478649944067</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.0013323083985596895</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.12575873732566833</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.026782017201185226</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.14786736667156219</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.0079238424077630043</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.0089279608801007271</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.0034250891767442226</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.19492627680301666</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.0013621053658425808</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.15700611472129822</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.0074168010614812374</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.0098066255450248718</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.0028364502359181643</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.17842809855937958</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.095474287867546082</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.12921270728111267</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.02707943320274353</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.018484009429812431</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.02013266459107399</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.29038310050964355</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.75850707292556763</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.093052171170711517</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.01492936909198761</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.009319760836660862</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.0077525991946458817</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.88356095552444458</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.091617211699485779</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.17878565192222595</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.022663945332169533</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.015142330899834633</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.013279451988637447</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.32148858904838562</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.072957605123519897</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.13023675978183746</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.0086859436705708504</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.0068710003979504108</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.00074462429620325565</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.21949593722820282</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.0013634042115882039</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.16474790871143341</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.0092125041410326958</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.0076129739172756672</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.00069281493779271841</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.1836296021938324</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.013937021605670452</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.078382425010204315</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.024353647604584694</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.017090862616896629</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.01990043930709362</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.15366439521312714</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.67860984802246094</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.06802792102098465</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.0096436068415641785</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.0074772806838154793</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.0059972428716719151</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.76975589990615845</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.018441857770085335</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.12177031487226486</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.017115481197834015</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.013159295544028282</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.0082943066954612732</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.17878125607967377</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C30" s="1">
         <v>0.04421113058924675</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D30" s="1">
         <v>0.048938345164060593</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E30" s="1">
         <v>0.0061555369757115841</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F30" s="1">
         <v>0.0010032366262748837</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G30" s="1">
         <v>0.0068663475103676319</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H30" s="1">
         <v>0.1071745976805687</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.00044024514500051737</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.036016292870044708</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.008463333360850811</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.00025547624682076275</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.009628642350435257</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.054803989827632904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>